<commit_message>
Changed MRP method to work with larger embedding sets (though now runs slower). Also built tables for new paper
</commit_message>
<xml_diff>
--- a/results/table_embed_sets/table_embed_sets.xlsx
+++ b/results/table_embed_sets/table_embed_sets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D426C22-7E60-4A37-8265-1F8434A54318}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25126105-FBB4-4003-91CA-0E3618AA5C6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="42">
   <si>
     <t>DeVine_etal_200.txt</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t>SysVec</t>
+  </si>
+  <si>
+    <t>embed p's</t>
+  </si>
+  <si>
+    <t>com p's</t>
+  </si>
+  <si>
+    <t>z-scores</t>
   </si>
 </sst>
 </file>
@@ -585,7 +594,7 @@
   <dimension ref="A1:BCF13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -65597,10 +65606,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93CD3AC9-9B9E-4EE1-99C0-6A6B29FB8DD3}">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:C34"/>
+      <selection activeCell="T19" sqref="T19:W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -66384,7 +66393,7 @@
         <v>9.9999999999999995E-8</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -66433,7 +66442,7 @@
         <v>89.000000099999994</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -66482,7 +66491,7 @@
         <v>25.000000100000001</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
         <v>30</v>
       </c>
@@ -66510,13 +66519,66 @@
         <f t="shared" si="6"/>
         <v>1093.0000016999998</v>
       </c>
+      <c r="T19" t="s">
+        <v>41</v>
+      </c>
+      <c r="U19">
+        <f>(M21-J21)/SQRT(J22*(1-J22)*(1/O19+1/O19))</f>
+        <v>19.026467127537536</v>
+      </c>
+      <c r="V19">
+        <f>(M21-K21)/SQRT(K22*(1-K22)*(1/O19+1/O19))</f>
+        <v>11.859071370306516</v>
+      </c>
+      <c r="W19">
+        <f>(M21-L21)/SQRT(L22*(1-L22)*(1/O19+1/O19))</f>
+        <v>11.817173613479291</v>
+      </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>39</v>
+      </c>
+      <c r="J21">
+        <f>J19/$O19</f>
+        <v>0.26715447383418434</v>
+      </c>
+      <c r="K21">
+        <f>K19/$O19</f>
+        <v>0.4208609788480781</v>
+      </c>
+      <c r="L21">
+        <f>L19/$O19</f>
+        <v>0.42177508687456305</v>
+      </c>
+      <c r="M21">
+        <f>M19/$O19</f>
+        <v>0.6733767793580564</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22">
+        <f>(J19+$M19)/($O19*2)</f>
+        <v>0.47026562659612031</v>
+      </c>
+      <c r="K22">
+        <f>(K19+$M19)/($O19*2)</f>
+        <v>0.54711887910306733</v>
+      </c>
+      <c r="L22">
+        <f>(L19+$M19)/($O19*2)</f>
+        <v>0.5475759331163097</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -66525,7 +66587,7 @@
         <v>0.26715447383418434</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -66534,7 +66596,7 @@
         <v>0.4208609788480781</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -66568,10 +66630,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28A33B2-E149-4F10-A439-500E5C0EE44F}">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:C34"/>
+      <selection activeCell="E48" sqref="D48:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -67355,7 +67417,7 @@
         <v>9.9999999999999995E-8</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -67404,7 +67466,7 @@
         <v>89.000000099999994</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -67453,7 +67515,7 @@
         <v>25.000000100000001</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
         <v>30</v>
       </c>
@@ -67481,13 +67543,66 @@
         <f t="shared" si="5"/>
         <v>1093.0000016999998</v>
       </c>
+      <c r="T19" t="s">
+        <v>41</v>
+      </c>
+      <c r="U19">
+        <f>(M21-J21)/SQRT(J22*(1-J22)*(1/O19+1/O19))</f>
+        <v>7.3353291574150807</v>
+      </c>
+      <c r="V19">
+        <f>(M21-K21)/SQRT(K22*(1-K22)*(1/O19+1/O19))</f>
+        <v>6.673051487507732</v>
+      </c>
+      <c r="W19">
+        <f>(M21-L21)/SQRT(L22*(1-L22)*(1/O19+1/O19))</f>
+        <v>9.6476105040417472</v>
+      </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>39</v>
+      </c>
+      <c r="J21">
+        <f>J19/$O19</f>
+        <v>0.78865077644949122</v>
+      </c>
+      <c r="K21">
+        <f>K19/$O19</f>
+        <v>0.8005417187914724</v>
+      </c>
+      <c r="L21">
+        <f>L19/$O19</f>
+        <v>0.74473064842997072</v>
+      </c>
+      <c r="M21">
+        <f>M19/$O19</f>
+        <v>0.9020970708750552</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22">
+        <f>(J19+$M19)/($O19*2)</f>
+        <v>0.84537392366227326</v>
+      </c>
+      <c r="K22">
+        <f>(K19+$M19)/($O19*2)</f>
+        <v>0.85131939483326391</v>
+      </c>
+      <c r="L22">
+        <f>(L19+$M19)/($O19*2)</f>
+        <v>0.8234138596525129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -67496,7 +67611,7 @@
         <v>0.78865077644949122</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -67505,7 +67620,7 @@
         <v>0.8005417187914724</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>

</xml_diff>